<commit_message>
update complaints, viewComplaints, snelzoeken.js, docs.
</commit_message>
<xml_diff>
--- a/documentation/ClassDiagram.xlsx
+++ b/documentation/ClassDiagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9A8CD9-47D0-4603-A924-C9F2D31F9748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43741FFD-46F1-44AB-91C2-4EDCD3A59069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{21C248FA-6220-4A7A-94FF-3E85FF0077CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Signup</t>
   </si>
@@ -168,6 +168,33 @@
   </si>
   <si>
     <t>[ - ] uid : String</t>
+  </si>
+  <si>
+    <t>Class Diagram</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>[ - ] host : String</t>
+  </si>
+  <si>
+    <t>[ - ] user : String</t>
+  </si>
+  <si>
+    <t>[ - ] passw : String</t>
+  </si>
+  <si>
+    <t>[ - ] db : String</t>
+  </si>
+  <si>
+    <t>[ - ] conn : String</t>
+  </si>
+  <si>
+    <t>[ - ] linkage() : void</t>
+  </si>
+  <si>
+    <t>[ # ] connect() : void</t>
   </si>
 </sst>
 </file>
@@ -198,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +244,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -319,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -342,7 +375,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -659,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3696BEB8-DDB4-4334-B10F-9789E88B1057}">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -695,13 +731,15 @@
     </row>
     <row r="2" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="1"/>
+      <c r="B2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -713,6 +751,15 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+    </row>
     <row r="5" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
         <v>7</v>
@@ -894,30 +941,69 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B22" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="H22" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="H23" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="H24" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="H25" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="H26" s="8"/>
     </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="8"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>